<commit_message>
Worked on the demos...
</commit_message>
<xml_diff>
--- a/_talks/but_we_dont_have_time/test_matrix.xlsx
+++ b/_talks/but_we_dont_have_time/test_matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -136,32 +136,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <b/>
@@ -179,6 +154,16 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -193,8 +178,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabelle3" displayName="Tabelle3" ref="A2:C11" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabelle3" displayName="Tabelle3" ref="A2:C11" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A2:C11"/>
+  <sortState ref="A3:C11">
+    <sortCondition ref="A2:A11"/>
+  </sortState>
   <tableColumns count="3">
     <tableColumn id="1" name="Protocol"/>
     <tableColumn id="2" name="Friend-State"/>
@@ -541,13 +529,13 @@
   <dimension ref="A2:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="3" max="3" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -567,15 +555,15 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -586,10 +574,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -597,7 +585,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -611,43 +599,43 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -663,10 +651,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:C11">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>EXACT(C3,"Die rebel scum!")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>EXACT(C3,"Welcome")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>